<commit_message>
Added 277 and 834 examples
</commit_message>
<xml_diff>
--- a/converted_files/834/834-all-fields.xlsx
+++ b/converted_files/834/834-all-fields.xlsx
@@ -59,7 +59,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:OZ5"/>
+  <dimension ref="A1:PD5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -533,1615 +533,1635 @@
       </c>
       <c r="CP1" s="3" t="inlineStr">
         <is>
+          <t>MemberLanguageInfoCodeQualifier</t>
+        </is>
+      </c>
+      <c r="CQ1" s="3" t="inlineStr">
+        <is>
+          <t>MemberLanguageInfoCode</t>
+        </is>
+      </c>
+      <c r="CR1" s="3" t="inlineStr">
+        <is>
+          <t>MemberLanguageInfoLanguageDescription</t>
+        </is>
+      </c>
+      <c r="CS1" s="3" t="inlineStr">
+        <is>
+          <t>MemberLanguageInfoLanguageUseIndicator</t>
+        </is>
+      </c>
+      <c r="CT1" s="3" t="inlineStr">
+        <is>
           <t>IncorrectMemberIdentifier</t>
         </is>
       </c>
-      <c r="CQ1" s="3" t="inlineStr">
+      <c r="CU1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberLastName</t>
         </is>
       </c>
-      <c r="CR1" s="3" t="inlineStr">
+      <c r="CV1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberFirstName</t>
         </is>
       </c>
-      <c r="CS1" s="3" t="inlineStr">
+      <c r="CW1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberMiddleName</t>
         </is>
       </c>
-      <c r="CT1" s="3" t="inlineStr">
+      <c r="CX1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberBirthDate</t>
         </is>
       </c>
-      <c r="CU1" s="3" t="inlineStr">
+      <c r="CY1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberGender</t>
         </is>
       </c>
-      <c r="CV1" s="3" t="inlineStr">
+      <c r="CZ1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberMaritalStatusCode</t>
         </is>
       </c>
-      <c r="CW1" s="3" t="inlineStr">
+      <c r="DA1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberEthnicityCode</t>
         </is>
       </c>
-      <c r="CX1" s="3" t="inlineStr">
+      <c r="DB1" s="3" t="inlineStr">
         <is>
           <t>IncorrectMemberCitizenshipCode</t>
         </is>
       </c>
-      <c r="CY1" s="3" t="inlineStr">
+      <c r="DC1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount1QualifierCode</t>
         </is>
       </c>
-      <c r="CZ1" s="3" t="inlineStr">
+      <c r="DD1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount1Amount</t>
         </is>
       </c>
-      <c r="DA1" s="3" t="inlineStr">
+      <c r="DE1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount2QualifierCode</t>
         </is>
       </c>
-      <c r="DB1" s="3" t="inlineStr">
+      <c r="DF1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount2Amount</t>
         </is>
       </c>
-      <c r="DC1" s="3" t="inlineStr">
+      <c r="DG1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount3QualifierCode</t>
         </is>
       </c>
-      <c r="DD1" s="3" t="inlineStr">
+      <c r="DH1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount3Amount</t>
         </is>
       </c>
-      <c r="DE1" s="3" t="inlineStr">
+      <c r="DI1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount4QualifierCode</t>
         </is>
       </c>
-      <c r="DF1" s="3" t="inlineStr">
+      <c r="DJ1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount4Amount</t>
         </is>
       </c>
-      <c r="DG1" s="3" t="inlineStr">
+      <c r="DK1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount5QualifierCode</t>
         </is>
       </c>
-      <c r="DH1" s="3" t="inlineStr">
+      <c r="DL1" s="3" t="inlineStr">
         <is>
           <t>ContractAmount5Amount</t>
         </is>
       </c>
-      <c r="DI1" s="3" t="inlineStr">
+      <c r="DM1" s="3" t="inlineStr">
         <is>
           <t>MailingAddressLine</t>
         </is>
       </c>
-      <c r="DJ1" s="3" t="inlineStr">
+      <c r="DN1" s="3" t="inlineStr">
         <is>
           <t>MailingAddressLine2</t>
         </is>
       </c>
-      <c r="DK1" s="3" t="inlineStr">
+      <c r="DO1" s="3" t="inlineStr">
         <is>
           <t>MailingAddressCity</t>
         </is>
       </c>
-      <c r="DL1" s="3" t="inlineStr">
+      <c r="DP1" s="3" t="inlineStr">
         <is>
           <t>MailingAddressStateCode</t>
         </is>
       </c>
-      <c r="DM1" s="3" t="inlineStr">
+      <c r="DQ1" s="3" t="inlineStr">
         <is>
           <t>MailingAddressZipCode</t>
         </is>
       </c>
-      <c r="DN1" s="3" t="inlineStr">
+      <c r="DR1" s="3" t="inlineStr">
         <is>
           <t>Employer1Identifier</t>
         </is>
       </c>
-      <c r="DO1" s="3" t="inlineStr">
+      <c r="DS1" s="3" t="inlineStr">
         <is>
           <t>Employer1LastNameOrOrgName</t>
         </is>
       </c>
-      <c r="DP1" s="3" t="inlineStr">
+      <c r="DT1" s="3" t="inlineStr">
         <is>
           <t>Employer1FirstName</t>
         </is>
       </c>
-      <c r="DQ1" s="3" t="inlineStr">
+      <c r="DU1" s="3" t="inlineStr">
         <is>
           <t>Employer1MiddleName</t>
         </is>
       </c>
-      <c r="DR1" s="3" t="inlineStr">
+      <c r="DV1" s="3" t="inlineStr">
         <is>
           <t>Employer1AddressLine</t>
         </is>
       </c>
-      <c r="DS1" s="3" t="inlineStr">
+      <c r="DW1" s="3" t="inlineStr">
         <is>
           <t>Employer1AddressLine2</t>
         </is>
       </c>
-      <c r="DT1" s="3" t="inlineStr">
+      <c r="DX1" s="3" t="inlineStr">
         <is>
           <t>Employer1AddressCity</t>
         </is>
       </c>
-      <c r="DU1" s="3" t="inlineStr">
+      <c r="DY1" s="3" t="inlineStr">
         <is>
           <t>Employer1AddressStateCode</t>
         </is>
       </c>
-      <c r="DV1" s="3" t="inlineStr">
+      <c r="DZ1" s="3" t="inlineStr">
         <is>
           <t>Employer1AddressZipCode</t>
         </is>
       </c>
-      <c r="DW1" s="3" t="inlineStr">
+      <c r="EA1" s="3" t="inlineStr">
         <is>
           <t>Employer1ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="DX1" s="3" t="inlineStr">
+      <c r="EB1" s="3" t="inlineStr">
         <is>
           <t>Employer1ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="DY1" s="3" t="inlineStr">
+      <c r="EC1" s="3" t="inlineStr">
         <is>
           <t>Employer1ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="DZ1" s="3" t="inlineStr">
+      <c r="ED1" s="3" t="inlineStr">
         <is>
           <t>Employer1ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="EA1" s="3" t="inlineStr">
+      <c r="EE1" s="3" t="inlineStr">
         <is>
           <t>Employer2Identifier</t>
         </is>
       </c>
-      <c r="EB1" s="3" t="inlineStr">
+      <c r="EF1" s="3" t="inlineStr">
         <is>
           <t>Employer2LastNameOrOrgName</t>
         </is>
       </c>
-      <c r="EC1" s="3" t="inlineStr">
+      <c r="EG1" s="3" t="inlineStr">
         <is>
           <t>Employer2FirstName</t>
         </is>
       </c>
-      <c r="ED1" s="3" t="inlineStr">
+      <c r="EH1" s="3" t="inlineStr">
         <is>
           <t>Employer2MiddleName</t>
         </is>
       </c>
-      <c r="EE1" s="3" t="inlineStr">
+      <c r="EI1" s="3" t="inlineStr">
         <is>
           <t>Employer2AddressLine</t>
         </is>
       </c>
-      <c r="EF1" s="3" t="inlineStr">
+      <c r="EJ1" s="3" t="inlineStr">
         <is>
           <t>Employer2AddressLine2</t>
         </is>
       </c>
-      <c r="EG1" s="3" t="inlineStr">
+      <c r="EK1" s="3" t="inlineStr">
         <is>
           <t>Employer2AddressCity</t>
         </is>
       </c>
-      <c r="EH1" s="3" t="inlineStr">
+      <c r="EL1" s="3" t="inlineStr">
         <is>
           <t>Employer2AddressStateCode</t>
         </is>
       </c>
-      <c r="EI1" s="3" t="inlineStr">
+      <c r="EM1" s="3" t="inlineStr">
         <is>
           <t>Employer2AddressZipCode</t>
         </is>
       </c>
-      <c r="EJ1" s="3" t="inlineStr">
+      <c r="EN1" s="3" t="inlineStr">
         <is>
           <t>Employer2ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="EK1" s="3" t="inlineStr">
+      <c r="EO1" s="3" t="inlineStr">
         <is>
           <t>Employer2ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="EL1" s="3" t="inlineStr">
+      <c r="EP1" s="3" t="inlineStr">
         <is>
           <t>Employer2ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="EM1" s="3" t="inlineStr">
+      <c r="EQ1" s="3" t="inlineStr">
         <is>
           <t>Employer2ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="EN1" s="3" t="inlineStr">
+      <c r="ER1" s="3" t="inlineStr">
         <is>
           <t>School1Identifier</t>
         </is>
       </c>
-      <c r="EO1" s="3" t="inlineStr">
+      <c r="ES1" s="3" t="inlineStr">
         <is>
           <t>School1Name</t>
         </is>
       </c>
-      <c r="EP1" s="3" t="inlineStr">
+      <c r="ET1" s="3" t="inlineStr">
         <is>
           <t>School1AddressLine</t>
         </is>
       </c>
-      <c r="EQ1" s="3" t="inlineStr">
+      <c r="EU1" s="3" t="inlineStr">
         <is>
           <t>School1AddressLine2</t>
         </is>
       </c>
-      <c r="ER1" s="3" t="inlineStr">
+      <c r="EV1" s="3" t="inlineStr">
         <is>
           <t>School1AddressCity</t>
         </is>
       </c>
-      <c r="ES1" s="3" t="inlineStr">
+      <c r="EW1" s="3" t="inlineStr">
         <is>
           <t>School1AddressStateCode</t>
         </is>
       </c>
-      <c r="ET1" s="3" t="inlineStr">
+      <c r="EX1" s="3" t="inlineStr">
         <is>
           <t>School1AddressZipCode</t>
         </is>
       </c>
-      <c r="EU1" s="3" t="inlineStr">
+      <c r="EY1" s="3" t="inlineStr">
         <is>
           <t>School1ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="EV1" s="3" t="inlineStr">
+      <c r="EZ1" s="3" t="inlineStr">
         <is>
           <t>School1ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="EW1" s="3" t="inlineStr">
+      <c r="FA1" s="3" t="inlineStr">
         <is>
           <t>School1ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="EX1" s="3" t="inlineStr">
+      <c r="FB1" s="3" t="inlineStr">
         <is>
           <t>School1ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="EY1" s="3" t="inlineStr">
+      <c r="FC1" s="3" t="inlineStr">
         <is>
           <t>School2Identifier</t>
         </is>
       </c>
-      <c r="EZ1" s="3" t="inlineStr">
+      <c r="FD1" s="3" t="inlineStr">
         <is>
           <t>School2Name</t>
         </is>
       </c>
-      <c r="FA1" s="3" t="inlineStr">
+      <c r="FE1" s="3" t="inlineStr">
         <is>
           <t>School2AddressLine</t>
         </is>
       </c>
-      <c r="FB1" s="3" t="inlineStr">
+      <c r="FF1" s="3" t="inlineStr">
         <is>
           <t>School2AddressLine2</t>
         </is>
       </c>
-      <c r="FC1" s="3" t="inlineStr">
+      <c r="FG1" s="3" t="inlineStr">
         <is>
           <t>School2AddressCity</t>
         </is>
       </c>
-      <c r="FD1" s="3" t="inlineStr">
+      <c r="FH1" s="3" t="inlineStr">
         <is>
           <t>School2AddressStateCode</t>
         </is>
       </c>
-      <c r="FE1" s="3" t="inlineStr">
+      <c r="FI1" s="3" t="inlineStr">
         <is>
           <t>School2AddressZipCode</t>
         </is>
       </c>
-      <c r="FF1" s="3" t="inlineStr">
+      <c r="FJ1" s="3" t="inlineStr">
         <is>
           <t>School2ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="FG1" s="3" t="inlineStr">
+      <c r="FK1" s="3" t="inlineStr">
         <is>
           <t>School2ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="FH1" s="3" t="inlineStr">
+      <c r="FL1" s="3" t="inlineStr">
         <is>
           <t>School2ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="FI1" s="3" t="inlineStr">
+      <c r="FM1" s="3" t="inlineStr">
         <is>
           <t>School2ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="FJ1" s="3" t="inlineStr">
+      <c r="FN1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentIdentifier</t>
         </is>
       </c>
-      <c r="FK1" s="3" t="inlineStr">
+      <c r="FO1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentLastName</t>
         </is>
       </c>
-      <c r="FL1" s="3" t="inlineStr">
+      <c r="FP1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentFirstName</t>
         </is>
       </c>
-      <c r="FM1" s="3" t="inlineStr">
+      <c r="FQ1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentMiddleName</t>
         </is>
       </c>
-      <c r="FN1" s="3" t="inlineStr">
+      <c r="FR1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentAddressLine</t>
         </is>
       </c>
-      <c r="FO1" s="3" t="inlineStr">
+      <c r="FS1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentAddressLine2</t>
         </is>
       </c>
-      <c r="FP1" s="3" t="inlineStr">
+      <c r="FT1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentAddressCity</t>
         </is>
       </c>
-      <c r="FQ1" s="3" t="inlineStr">
+      <c r="FU1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentAddressStateCode</t>
         </is>
       </c>
-      <c r="FR1" s="3" t="inlineStr">
+      <c r="FV1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentAddressZipCode</t>
         </is>
       </c>
-      <c r="FS1" s="3" t="inlineStr">
+      <c r="FW1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="FT1" s="3" t="inlineStr">
+      <c r="FX1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="FU1" s="3" t="inlineStr">
+      <c r="FY1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="FV1" s="3" t="inlineStr">
+      <c r="FZ1" s="3" t="inlineStr">
         <is>
           <t>CustodialParentContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="FW1" s="3" t="inlineStr">
+      <c r="GA1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1EntityRole</t>
         </is>
       </c>
-      <c r="FX1" s="3" t="inlineStr">
+      <c r="GB1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1Identifier</t>
         </is>
       </c>
-      <c r="FY1" s="3" t="inlineStr">
+      <c r="GC1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1LastName</t>
         </is>
       </c>
-      <c r="FZ1" s="3" t="inlineStr">
+      <c r="GD1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1FirstName</t>
         </is>
       </c>
-      <c r="GA1" s="3" t="inlineStr">
+      <c r="GE1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1MiddleName</t>
         </is>
       </c>
-      <c r="GB1" s="3" t="inlineStr">
+      <c r="GF1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1AddressLine</t>
         </is>
       </c>
-      <c r="GC1" s="3" t="inlineStr">
+      <c r="GG1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1AddressLine2</t>
         </is>
       </c>
-      <c r="GD1" s="3" t="inlineStr">
+      <c r="GH1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1AddressCity</t>
         </is>
       </c>
-      <c r="GE1" s="3" t="inlineStr">
+      <c r="GI1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1AddressStateCode</t>
         </is>
       </c>
-      <c r="GF1" s="3" t="inlineStr">
+      <c r="GJ1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1AddressZipCode</t>
         </is>
       </c>
-      <c r="GG1" s="3" t="inlineStr">
+      <c r="GK1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="GH1" s="3" t="inlineStr">
+      <c r="GL1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="GI1" s="3" t="inlineStr">
+      <c r="GM1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="GJ1" s="3" t="inlineStr">
+      <c r="GN1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson1ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="GK1" s="3" t="inlineStr">
+      <c r="GO1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2EntityRole</t>
         </is>
       </c>
-      <c r="GL1" s="3" t="inlineStr">
+      <c r="GP1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2Identifier</t>
         </is>
       </c>
-      <c r="GM1" s="3" t="inlineStr">
+      <c r="GQ1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2LastName</t>
         </is>
       </c>
-      <c r="GN1" s="3" t="inlineStr">
+      <c r="GR1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2FirstName</t>
         </is>
       </c>
-      <c r="GO1" s="3" t="inlineStr">
+      <c r="GS1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2MiddleName</t>
         </is>
       </c>
-      <c r="GP1" s="3" t="inlineStr">
+      <c r="GT1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2AddressLine</t>
         </is>
       </c>
-      <c r="GQ1" s="3" t="inlineStr">
+      <c r="GU1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2AddressLine2</t>
         </is>
       </c>
-      <c r="GR1" s="3" t="inlineStr">
+      <c r="GV1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2AddressCity</t>
         </is>
       </c>
-      <c r="GS1" s="3" t="inlineStr">
+      <c r="GW1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2AddressStateCode</t>
         </is>
       </c>
-      <c r="GT1" s="3" t="inlineStr">
+      <c r="GX1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2AddressZipCode</t>
         </is>
       </c>
-      <c r="GU1" s="3" t="inlineStr">
+      <c r="GY1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="GV1" s="3" t="inlineStr">
+      <c r="GZ1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="GW1" s="3" t="inlineStr">
+      <c r="HA1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="GX1" s="3" t="inlineStr">
+      <c r="HB1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson2ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="GY1" s="3" t="inlineStr">
+      <c r="HC1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3EntityRole</t>
         </is>
       </c>
-      <c r="GZ1" s="3" t="inlineStr">
+      <c r="HD1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3Identifier</t>
         </is>
       </c>
-      <c r="HA1" s="3" t="inlineStr">
+      <c r="HE1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3LastName</t>
         </is>
       </c>
-      <c r="HB1" s="3" t="inlineStr">
+      <c r="HF1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3FirstName</t>
         </is>
       </c>
-      <c r="HC1" s="3" t="inlineStr">
+      <c r="HG1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3MiddleName</t>
         </is>
       </c>
-      <c r="HD1" s="3" t="inlineStr">
+      <c r="HH1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3AddressLine</t>
         </is>
       </c>
-      <c r="HE1" s="3" t="inlineStr">
+      <c r="HI1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3AddressLine2</t>
         </is>
       </c>
-      <c r="HF1" s="3" t="inlineStr">
+      <c r="HJ1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3AddressCity</t>
         </is>
       </c>
-      <c r="HG1" s="3" t="inlineStr">
+      <c r="HK1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3AddressStateCode</t>
         </is>
       </c>
-      <c r="HH1" s="3" t="inlineStr">
+      <c r="HL1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3AddressZipCode</t>
         </is>
       </c>
-      <c r="HI1" s="3" t="inlineStr">
+      <c r="HM1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="HJ1" s="3" t="inlineStr">
+      <c r="HN1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="HK1" s="3" t="inlineStr">
+      <c r="HO1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="HL1" s="3" t="inlineStr">
+      <c r="HP1" s="3" t="inlineStr">
         <is>
           <t>ResponsiblePerson3ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="HM1" s="3" t="inlineStr">
+      <c r="HQ1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationLastNameOrOrgName</t>
         </is>
       </c>
-      <c r="HN1" s="3" t="inlineStr">
+      <c r="HR1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationFirstName</t>
         </is>
       </c>
-      <c r="HO1" s="3" t="inlineStr">
+      <c r="HS1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationMiddleName</t>
         </is>
       </c>
-      <c r="HP1" s="3" t="inlineStr">
+      <c r="HT1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationAddressLine</t>
         </is>
       </c>
-      <c r="HQ1" s="3" t="inlineStr">
+      <c r="HU1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationAddressLine2</t>
         </is>
       </c>
-      <c r="HR1" s="3" t="inlineStr">
+      <c r="HV1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationAddressCity</t>
         </is>
       </c>
-      <c r="HS1" s="3" t="inlineStr">
+      <c r="HW1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationAddressStateCode</t>
         </is>
       </c>
-      <c r="HT1" s="3" t="inlineStr">
+      <c r="HX1" s="3" t="inlineStr">
         <is>
           <t>DropOffLocationAddressZipCode</t>
         </is>
       </c>
-      <c r="HU1" s="3" t="inlineStr">
+      <c r="HY1" s="3" t="inlineStr">
         <is>
           <t>Disability1TypeCode</t>
         </is>
       </c>
-      <c r="HV1" s="3" t="inlineStr">
+      <c r="HZ1" s="3" t="inlineStr">
         <is>
           <t>Disability1DiagnosisCode</t>
         </is>
       </c>
-      <c r="HW1" s="3" t="inlineStr">
+      <c r="IA1" s="3" t="inlineStr">
         <is>
           <t>Disability1DateFrom</t>
         </is>
       </c>
-      <c r="HX1" s="3" t="inlineStr">
+      <c r="IB1" s="3" t="inlineStr">
         <is>
           <t>Disability1DateTo</t>
         </is>
       </c>
-      <c r="HY1" s="3" t="inlineStr">
+      <c r="IC1" s="3" t="inlineStr">
         <is>
           <t>Disability2TypeCode</t>
         </is>
       </c>
-      <c r="HZ1" s="3" t="inlineStr">
+      <c r="ID1" s="3" t="inlineStr">
         <is>
           <t>Disability2DiagnosisCode</t>
         </is>
       </c>
-      <c r="IA1" s="3" t="inlineStr">
+      <c r="IE1" s="3" t="inlineStr">
         <is>
           <t>Disability2DateFrom</t>
         </is>
       </c>
-      <c r="IB1" s="3" t="inlineStr">
+      <c r="IF1" s="3" t="inlineStr">
         <is>
           <t>Disability2DateTo</t>
         </is>
       </c>
-      <c r="IC1" s="3" t="inlineStr">
+      <c r="IG1" s="3" t="inlineStr">
         <is>
           <t>Disability3TypeCode</t>
         </is>
       </c>
-      <c r="ID1" s="3" t="inlineStr">
+      <c r="IH1" s="3" t="inlineStr">
         <is>
           <t>Disability3DiagnosisCode</t>
         </is>
       </c>
-      <c r="IE1" s="3" t="inlineStr">
+      <c r="II1" s="3" t="inlineStr">
         <is>
           <t>Disability3DateFrom</t>
         </is>
       </c>
-      <c r="IF1" s="3" t="inlineStr">
+      <c r="IJ1" s="3" t="inlineStr">
         <is>
           <t>Disability3DateTo</t>
         </is>
       </c>
-      <c r="IG1" s="3" t="inlineStr">
+      <c r="IK1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory1Name</t>
         </is>
       </c>
-      <c r="IH1" s="3" t="inlineStr">
+      <c r="IL1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory1IdentifierQualifierCode</t>
         </is>
       </c>
-      <c r="II1" s="3" t="inlineStr">
+      <c r="IM1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory1IdentifierType</t>
         </is>
       </c>
-      <c r="IJ1" s="3" t="inlineStr">
+      <c r="IN1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory1Identifier</t>
         </is>
       </c>
-      <c r="IK1" s="3" t="inlineStr">
+      <c r="IO1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory1Date</t>
         </is>
       </c>
-      <c r="IL1" s="3" t="inlineStr">
+      <c r="IP1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory1DateTo</t>
         </is>
       </c>
-      <c r="IM1" s="3" t="inlineStr">
+      <c r="IQ1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory2Name</t>
         </is>
       </c>
-      <c r="IN1" s="3" t="inlineStr">
+      <c r="IR1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory2IdentifierQualifierCode</t>
         </is>
       </c>
-      <c r="IO1" s="3" t="inlineStr">
+      <c r="IS1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory2IdentifierType</t>
         </is>
       </c>
-      <c r="IP1" s="3" t="inlineStr">
+      <c r="IT1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory2Identifier</t>
         </is>
       </c>
-      <c r="IQ1" s="3" t="inlineStr">
+      <c r="IU1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory2Date</t>
         </is>
       </c>
-      <c r="IR1" s="3" t="inlineStr">
+      <c r="IV1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory2DateTo</t>
         </is>
       </c>
-      <c r="IS1" s="3" t="inlineStr">
+      <c r="IW1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory3Name</t>
         </is>
       </c>
-      <c r="IT1" s="3" t="inlineStr">
+      <c r="IX1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory3IdentifierQualifierCode</t>
         </is>
       </c>
-      <c r="IU1" s="3" t="inlineStr">
+      <c r="IY1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory3IdentifierType</t>
         </is>
       </c>
-      <c r="IV1" s="3" t="inlineStr">
+      <c r="IZ1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory3Identifier</t>
         </is>
       </c>
-      <c r="IW1" s="3" t="inlineStr">
+      <c r="JA1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory3Date</t>
         </is>
       </c>
-      <c r="IX1" s="3" t="inlineStr">
+      <c r="JB1" s="3" t="inlineStr">
         <is>
           <t>ReportingCategory3DateTo</t>
         </is>
       </c>
-      <c r="IY1" s="3" t="inlineStr">
+      <c r="JC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageMaintenanceTypeCode</t>
         </is>
       </c>
-      <c r="IZ1" s="3" t="inlineStr">
+      <c r="JD1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageInsuranceLineCode</t>
         </is>
       </c>
-      <c r="JA1" s="3" t="inlineStr">
+      <c r="JE1" s="3" t="inlineStr">
         <is>
           <t>HealthCoveragePlanDescription</t>
         </is>
       </c>
-      <c r="JB1" s="3" t="inlineStr">
+      <c r="JF1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageLevelCode</t>
         </is>
       </c>
-      <c r="JC1" s="3" t="inlineStr">
+      <c r="JG1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageLateEnrollmentIndicator</t>
         </is>
       </c>
-      <c r="JD1" s="3" t="inlineStr">
+      <c r="JH1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate1QualifierCode</t>
         </is>
       </c>
-      <c r="JE1" s="3" t="inlineStr">
+      <c r="JI1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate1Date</t>
         </is>
       </c>
-      <c r="JF1" s="3" t="inlineStr">
+      <c r="JJ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate2QualifierCode</t>
         </is>
       </c>
-      <c r="JG1" s="3" t="inlineStr">
+      <c r="JK1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate2Date</t>
         </is>
       </c>
-      <c r="JH1" s="3" t="inlineStr">
+      <c r="JL1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate3QualifierCode</t>
         </is>
       </c>
-      <c r="JI1" s="3" t="inlineStr">
+      <c r="JM1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate3Date</t>
         </is>
       </c>
-      <c r="JJ1" s="3" t="inlineStr">
+      <c r="JN1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate4QualifierCode</t>
         </is>
       </c>
-      <c r="JK1" s="3" t="inlineStr">
+      <c r="JO1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate4Date</t>
         </is>
       </c>
-      <c r="JL1" s="3" t="inlineStr">
+      <c r="JP1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate5QualifierCode</t>
         </is>
       </c>
-      <c r="JM1" s="3" t="inlineStr">
+      <c r="JQ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCoverageDate5Date</t>
         </is>
       </c>
-      <c r="JN1" s="3" t="inlineStr">
+      <c r="JR1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageContractAmount1QualifierCode</t>
         </is>
       </c>
-      <c r="JO1" s="3" t="inlineStr">
+      <c r="JS1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageContractAmount1Amount</t>
         </is>
       </c>
-      <c r="JP1" s="3" t="inlineStr">
+      <c r="JT1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageContractAmount2QualifierCode</t>
         </is>
       </c>
-      <c r="JQ1" s="3" t="inlineStr">
+      <c r="JU1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageContractAmount2Amount</t>
         </is>
       </c>
-      <c r="JR1" s="3" t="inlineStr">
+      <c r="JV1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageContractAmount3QualifierCode</t>
         </is>
       </c>
-      <c r="JS1" s="3" t="inlineStr">
+      <c r="JW1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageContractAmount3Amount</t>
         </is>
       </c>
-      <c r="JT1" s="3" t="inlineStr">
+      <c r="JX1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber1QualifierCode</t>
         </is>
       </c>
-      <c r="JU1" s="3" t="inlineStr">
+      <c r="JY1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber1Identification</t>
         </is>
       </c>
-      <c r="JV1" s="3" t="inlineStr">
+      <c r="JZ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber2QualifierCode</t>
         </is>
       </c>
-      <c r="JW1" s="3" t="inlineStr">
+      <c r="KA1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber2Identification</t>
         </is>
       </c>
-      <c r="JX1" s="3" t="inlineStr">
+      <c r="KB1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber3QualifierCode</t>
         </is>
       </c>
-      <c r="JY1" s="3" t="inlineStr">
+      <c r="KC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber3Identification</t>
         </is>
       </c>
-      <c r="JZ1" s="3" t="inlineStr">
+      <c r="KD1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber4QualifierCode</t>
         </is>
       </c>
-      <c r="KA1" s="3" t="inlineStr">
+      <c r="KE1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber4Identification</t>
         </is>
       </c>
-      <c r="KB1" s="3" t="inlineStr">
+      <c r="KF1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber5QualifierCode</t>
         </is>
       </c>
-      <c r="KC1" s="3" t="inlineStr">
+      <c r="KG1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageGroupOrPolicyNumber5Identification</t>
         </is>
       </c>
-      <c r="KD1" s="3" t="inlineStr">
+      <c r="KH1" s="3" t="inlineStr">
         <is>
           <t>HealthCoveragePriorCoverageMonthCount</t>
         </is>
       </c>
-      <c r="KE1" s="3" t="inlineStr">
+      <c r="KI1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageIdCardPlanDesc</t>
         </is>
       </c>
-      <c r="KF1" s="3" t="inlineStr">
+      <c r="KJ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageIdCardTypeCode</t>
         </is>
       </c>
-      <c r="KG1" s="3" t="inlineStr">
+      <c r="KK1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageIdCardCount</t>
         </is>
       </c>
-      <c r="KH1" s="3" t="inlineStr">
+      <c r="KL1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageIdCardActionCode</t>
         </is>
       </c>
-      <c r="KI1" s="3" t="inlineStr">
+      <c r="KM1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1EntityRole</t>
         </is>
       </c>
-      <c r="KJ1" s="3" t="inlineStr">
+      <c r="KN1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1EntityType</t>
         </is>
       </c>
-      <c r="KK1" s="3" t="inlineStr">
+      <c r="KO1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1Identifier</t>
         </is>
       </c>
-      <c r="KL1" s="3" t="inlineStr">
+      <c r="KP1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1LastNameOrOrgName</t>
         </is>
       </c>
-      <c r="KM1" s="3" t="inlineStr">
+      <c r="KQ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1FirstName</t>
         </is>
       </c>
-      <c r="KN1" s="3" t="inlineStr">
+      <c r="KR1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1MiddleName</t>
         </is>
       </c>
-      <c r="KO1" s="3" t="inlineStr">
+      <c r="KS1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1AddressLine</t>
         </is>
       </c>
-      <c r="KP1" s="3" t="inlineStr">
+      <c r="KT1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1AddressLine2</t>
         </is>
       </c>
-      <c r="KQ1" s="3" t="inlineStr">
+      <c r="KU1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1AddressCity</t>
         </is>
       </c>
-      <c r="KR1" s="3" t="inlineStr">
+      <c r="KV1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1AddressStateCode</t>
         </is>
       </c>
-      <c r="KS1" s="3" t="inlineStr">
+      <c r="KW1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1AddressZipCode</t>
         </is>
       </c>
-      <c r="KT1" s="3" t="inlineStr">
+      <c r="KX1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="KU1" s="3" t="inlineStr">
+      <c r="KY1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="KV1" s="3" t="inlineStr">
+      <c r="KZ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="KW1" s="3" t="inlineStr">
+      <c r="LA1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="KX1" s="3" t="inlineStr">
+      <c r="LB1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ChangeReasonActionCode</t>
         </is>
       </c>
-      <c r="KY1" s="3" t="inlineStr">
+      <c r="LC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ChangeReasonEffectiveDate</t>
         </is>
       </c>
-      <c r="KZ1" s="3" t="inlineStr">
+      <c r="LD1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider1ChangeReasonReasonCode</t>
         </is>
       </c>
-      <c r="LA1" s="3" t="inlineStr">
+      <c r="LE1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2EntityRole</t>
         </is>
       </c>
-      <c r="LB1" s="3" t="inlineStr">
+      <c r="LF1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2EntityType</t>
         </is>
       </c>
-      <c r="LC1" s="3" t="inlineStr">
+      <c r="LG1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2Identifier</t>
         </is>
       </c>
-      <c r="LD1" s="3" t="inlineStr">
+      <c r="LH1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2LastNameOrOrgName</t>
         </is>
       </c>
-      <c r="LE1" s="3" t="inlineStr">
+      <c r="LI1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2FirstName</t>
         </is>
       </c>
-      <c r="LF1" s="3" t="inlineStr">
+      <c r="LJ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2MiddleName</t>
         </is>
       </c>
-      <c r="LG1" s="3" t="inlineStr">
+      <c r="LK1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2AddressLine</t>
         </is>
       </c>
-      <c r="LH1" s="3" t="inlineStr">
+      <c r="LL1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2AddressLine2</t>
         </is>
       </c>
-      <c r="LI1" s="3" t="inlineStr">
+      <c r="LM1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2AddressCity</t>
         </is>
       </c>
-      <c r="LJ1" s="3" t="inlineStr">
+      <c r="LN1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2AddressStateCode</t>
         </is>
       </c>
-      <c r="LK1" s="3" t="inlineStr">
+      <c r="LO1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2AddressZipCode</t>
         </is>
       </c>
-      <c r="LL1" s="3" t="inlineStr">
+      <c r="LP1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="LM1" s="3" t="inlineStr">
+      <c r="LQ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="LN1" s="3" t="inlineStr">
+      <c r="LR1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="LO1" s="3" t="inlineStr">
+      <c r="LS1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="LP1" s="3" t="inlineStr">
+      <c r="LT1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ChangeReasonActionCode</t>
         </is>
       </c>
-      <c r="LQ1" s="3" t="inlineStr">
+      <c r="LU1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ChangeReasonEffectiveDate</t>
         </is>
       </c>
-      <c r="LR1" s="3" t="inlineStr">
+      <c r="LV1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider2ChangeReasonReasonCode</t>
         </is>
       </c>
-      <c r="LS1" s="3" t="inlineStr">
+      <c r="LW1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3EntityRole</t>
         </is>
       </c>
-      <c r="LT1" s="3" t="inlineStr">
+      <c r="LX1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3EntityType</t>
         </is>
       </c>
-      <c r="LU1" s="3" t="inlineStr">
+      <c r="LY1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3Identifier</t>
         </is>
       </c>
-      <c r="LV1" s="3" t="inlineStr">
+      <c r="LZ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3LastNameOrOrgName</t>
         </is>
       </c>
-      <c r="LW1" s="3" t="inlineStr">
+      <c r="MA1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3FirstName</t>
         </is>
       </c>
-      <c r="LX1" s="3" t="inlineStr">
+      <c r="MB1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3MiddleName</t>
         </is>
       </c>
-      <c r="LY1" s="3" t="inlineStr">
+      <c r="MC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3AddressLine</t>
         </is>
       </c>
-      <c r="LZ1" s="3" t="inlineStr">
+      <c r="MD1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3AddressLine2</t>
         </is>
       </c>
-      <c r="MA1" s="3" t="inlineStr">
+      <c r="ME1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3AddressCity</t>
         </is>
       </c>
-      <c r="MB1" s="3" t="inlineStr">
+      <c r="MF1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3AddressStateCode</t>
         </is>
       </c>
-      <c r="MC1" s="3" t="inlineStr">
+      <c r="MG1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3AddressZipCode</t>
         </is>
       </c>
-      <c r="MD1" s="3" t="inlineStr">
+      <c r="MH1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="ME1" s="3" t="inlineStr">
+      <c r="MI1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="MF1" s="3" t="inlineStr">
+      <c r="MJ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="MG1" s="3" t="inlineStr">
+      <c r="MK1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="MH1" s="3" t="inlineStr">
+      <c r="ML1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ChangeReasonActionCode</t>
         </is>
       </c>
-      <c r="MI1" s="3" t="inlineStr">
+      <c r="MM1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ChangeReasonEffectiveDate</t>
         </is>
       </c>
-      <c r="MJ1" s="3" t="inlineStr">
+      <c r="MN1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageProvider3ChangeReasonReasonCode</t>
         </is>
       </c>
-      <c r="MK1" s="3" t="inlineStr">
+      <c r="MO1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1PayerResponsibilitySequenceCode</t>
         </is>
       </c>
-      <c r="ML1" s="3" t="inlineStr">
+      <c r="MP1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1PayerResponsibilitySequence</t>
         </is>
       </c>
-      <c r="MM1" s="3" t="inlineStr">
+      <c r="MQ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1GroupOrPolicyNumber</t>
         </is>
       </c>
-      <c r="MN1" s="3" t="inlineStr">
+      <c r="MR1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1CoordinationOfBenefitsCode</t>
         </is>
       </c>
-      <c r="MO1" s="3" t="inlineStr">
+      <c r="MS1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1AdditionalIdentifier1QualifierCode</t>
         </is>
       </c>
-      <c r="MP1" s="3" t="inlineStr">
+      <c r="MT1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1AdditionalIdentifier1Identification</t>
         </is>
       </c>
-      <c r="MQ1" s="3" t="inlineStr">
+      <c r="MU1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1AdditionalIdentifier2QualifierCode</t>
         </is>
       </c>
-      <c r="MR1" s="3" t="inlineStr">
+      <c r="MV1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1AdditionalIdentifier2Identification</t>
         </is>
       </c>
-      <c r="MS1" s="3" t="inlineStr">
+      <c r="MW1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1DateFrom</t>
         </is>
       </c>
-      <c r="MT1" s="3" t="inlineStr">
+      <c r="MX1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1DateTo</t>
         </is>
       </c>
-      <c r="MU1" s="3" t="inlineStr">
+      <c r="MY1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1EntityRole</t>
         </is>
       </c>
-      <c r="MV1" s="3" t="inlineStr">
+      <c r="MZ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1Identifier</t>
         </is>
       </c>
-      <c r="MW1" s="3" t="inlineStr">
+      <c r="NA1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1Name</t>
         </is>
       </c>
-      <c r="MX1" s="3" t="inlineStr">
+      <c r="NB1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1AddressLine</t>
         </is>
       </c>
-      <c r="MY1" s="3" t="inlineStr">
+      <c r="NC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1AddressLine2</t>
         </is>
       </c>
-      <c r="MZ1" s="3" t="inlineStr">
+      <c r="ND1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1AddressCity</t>
         </is>
       </c>
-      <c r="NA1" s="3" t="inlineStr">
+      <c r="NE1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1AddressStateCode</t>
         </is>
       </c>
-      <c r="NB1" s="3" t="inlineStr">
+      <c r="NF1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1AddressZipCode</t>
         </is>
       </c>
-      <c r="NC1" s="3" t="inlineStr">
+      <c r="NG1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="ND1" s="3" t="inlineStr">
+      <c r="NH1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="NE1" s="3" t="inlineStr">
+      <c r="NI1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="NF1" s="3" t="inlineStr">
+      <c r="NJ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer1ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="NG1" s="3" t="inlineStr">
+      <c r="NK1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2EntityRole</t>
         </is>
       </c>
-      <c r="NH1" s="3" t="inlineStr">
+      <c r="NL1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2Identifier</t>
         </is>
       </c>
-      <c r="NI1" s="3" t="inlineStr">
+      <c r="NM1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2Name</t>
         </is>
       </c>
-      <c r="NJ1" s="3" t="inlineStr">
+      <c r="NN1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2AddressLine</t>
         </is>
       </c>
-      <c r="NK1" s="3" t="inlineStr">
+      <c r="NO1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2AddressLine2</t>
         </is>
       </c>
-      <c r="NL1" s="3" t="inlineStr">
+      <c r="NP1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2AddressCity</t>
         </is>
       </c>
-      <c r="NM1" s="3" t="inlineStr">
+      <c r="NQ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2AddressStateCode</t>
         </is>
       </c>
-      <c r="NN1" s="3" t="inlineStr">
+      <c r="NR1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2AddressZipCode</t>
         </is>
       </c>
-      <c r="NO1" s="3" t="inlineStr">
+      <c r="NS1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="NP1" s="3" t="inlineStr">
+      <c r="NT1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="NQ1" s="3" t="inlineStr">
+      <c r="NU1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="NR1" s="3" t="inlineStr">
+      <c r="NV1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob1Insurer2ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="NS1" s="3" t="inlineStr">
+      <c r="NW1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2PayerResponsibilitySequenceCode</t>
         </is>
       </c>
-      <c r="NT1" s="3" t="inlineStr">
+      <c r="NX1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2PayerResponsibilitySequence</t>
         </is>
       </c>
-      <c r="NU1" s="3" t="inlineStr">
+      <c r="NY1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2GroupOrPolicyNumber</t>
         </is>
       </c>
-      <c r="NV1" s="3" t="inlineStr">
+      <c r="NZ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2CoordinationOfBenefitsCode</t>
         </is>
       </c>
-      <c r="NW1" s="3" t="inlineStr">
+      <c r="OA1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2AdditionalIdentifier1QualifierCode</t>
         </is>
       </c>
-      <c r="NX1" s="3" t="inlineStr">
+      <c r="OB1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2AdditionalIdentifier1Identification</t>
         </is>
       </c>
-      <c r="NY1" s="3" t="inlineStr">
+      <c r="OC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2AdditionalIdentifier2QualifierCode</t>
         </is>
       </c>
-      <c r="NZ1" s="3" t="inlineStr">
+      <c r="OD1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2AdditionalIdentifier2Identification</t>
         </is>
       </c>
-      <c r="OA1" s="3" t="inlineStr">
+      <c r="OE1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2DateFrom</t>
         </is>
       </c>
-      <c r="OB1" s="3" t="inlineStr">
+      <c r="OF1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2DateTo</t>
         </is>
       </c>
-      <c r="OC1" s="3" t="inlineStr">
+      <c r="OG1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1EntityRole</t>
         </is>
       </c>
-      <c r="OD1" s="3" t="inlineStr">
+      <c r="OH1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1Identifier</t>
         </is>
       </c>
-      <c r="OE1" s="3" t="inlineStr">
+      <c r="OI1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1Name</t>
         </is>
       </c>
-      <c r="OF1" s="3" t="inlineStr">
+      <c r="OJ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1AddressLine</t>
         </is>
       </c>
-      <c r="OG1" s="3" t="inlineStr">
+      <c r="OK1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1AddressLine2</t>
         </is>
       </c>
-      <c r="OH1" s="3" t="inlineStr">
+      <c r="OL1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1AddressCity</t>
         </is>
       </c>
-      <c r="OI1" s="3" t="inlineStr">
+      <c r="OM1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1AddressStateCode</t>
         </is>
       </c>
-      <c r="OJ1" s="3" t="inlineStr">
+      <c r="ON1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1AddressZipCode</t>
         </is>
       </c>
-      <c r="OK1" s="3" t="inlineStr">
+      <c r="OO1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="OL1" s="3" t="inlineStr">
+      <c r="OP1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="OM1" s="3" t="inlineStr">
+      <c r="OQ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="ON1" s="3" t="inlineStr">
+      <c r="OR1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer1ContactContactNumber2Number</t>
         </is>
       </c>
-      <c r="OO1" s="3" t="inlineStr">
+      <c r="OS1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2EntityRole</t>
         </is>
       </c>
-      <c r="OP1" s="3" t="inlineStr">
+      <c r="OT1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2Identifier</t>
         </is>
       </c>
-      <c r="OQ1" s="3" t="inlineStr">
+      <c r="OU1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2Name</t>
         </is>
       </c>
-      <c r="OR1" s="3" t="inlineStr">
+      <c r="OV1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2AddressLine</t>
         </is>
       </c>
-      <c r="OS1" s="3" t="inlineStr">
+      <c r="OW1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2AddressLine2</t>
         </is>
       </c>
-      <c r="OT1" s="3" t="inlineStr">
+      <c r="OX1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2AddressCity</t>
         </is>
       </c>
-      <c r="OU1" s="3" t="inlineStr">
+      <c r="OY1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2AddressStateCode</t>
         </is>
       </c>
-      <c r="OV1" s="3" t="inlineStr">
+      <c r="OZ1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2AddressZipCode</t>
         </is>
       </c>
-      <c r="OW1" s="3" t="inlineStr">
+      <c r="PA1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2ContactContactNumber1Type</t>
         </is>
       </c>
-      <c r="OX1" s="3" t="inlineStr">
+      <c r="PB1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2ContactContactNumber1Number</t>
         </is>
       </c>
-      <c r="OY1" s="3" t="inlineStr">
+      <c r="PC1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2ContactContactNumber2Type</t>
         </is>
       </c>
-      <c r="OZ1" s="3" t="inlineStr">
+      <c r="PD1" s="3" t="inlineStr">
         <is>
           <t>HealthCoverageCob2Insurer2ContactContactNumber2Number</t>
         </is>
@@ -2150,7 +2170,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>684723f4cd41c01c2437b822</t>
+          <t>685d5721e29351212dc46be9</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -2497,147 +2517,147 @@
       <c r="CO2" t="n">
         <v>210.0</v>
       </c>
-      <c r="CP2" s="3" t="inlineStr">
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2" s="3" t="inlineStr">
         <is>
           <t>202443309</t>
         </is>
       </c>
-      <c r="CQ2" s="3" t="inlineStr">
+      <c r="CU2" s="3" t="inlineStr">
         <is>
           <t>DOE</t>
         </is>
       </c>
-      <c r="CR2" s="3" t="inlineStr">
+      <c r="CV2" s="3" t="inlineStr">
         <is>
           <t>JOE</t>
         </is>
       </c>
-      <c r="CS2"/>
-      <c r="CT2" s="4" t="n">
+      <c r="CW2"/>
+      <c r="CX2" s="4" t="n">
         <v>25733.0</v>
       </c>
-      <c r="CU2" s="3" t="inlineStr">
+      <c r="CY2" s="3" t="inlineStr">
         <is>
           <t>MALE</t>
         </is>
       </c>
-      <c r="CV2" s="3" t="inlineStr">
+      <c r="CZ2" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="CW2" s="3" t="inlineStr">
+      <c r="DA2" s="3" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="CX2" s="3" t="inlineStr">
+      <c r="DB2" s="3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="CY2" s="3" t="inlineStr">
+      <c r="DC2" s="3" t="inlineStr">
         <is>
           <t>D2</t>
         </is>
       </c>
-      <c r="CZ2" s="1" t="n">
+      <c r="DD2" s="1" t="n">
         <v>100.0</v>
       </c>
-      <c r="DA2"/>
-      <c r="DB2"/>
-      <c r="DC2"/>
-      <c r="DD2"/>
       <c r="DE2"/>
       <c r="DF2"/>
       <c r="DG2"/>
       <c r="DH2"/>
-      <c r="DI2" s="3" t="inlineStr">
+      <c r="DI2"/>
+      <c r="DJ2"/>
+      <c r="DK2"/>
+      <c r="DL2"/>
+      <c r="DM2" s="3" t="inlineStr">
         <is>
           <t>9715 SOUTHWIND AVENUE</t>
         </is>
       </c>
-      <c r="DJ2"/>
-      <c r="DK2" s="3" t="inlineStr">
+      <c r="DN2"/>
+      <c r="DO2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="DL2" s="3" t="inlineStr">
+      <c r="DP2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="DM2" s="3" t="inlineStr">
+      <c r="DQ2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="DN2" s="3" t="inlineStr">
+      <c r="DR2" s="3" t="inlineStr">
         <is>
           <t>emp1ID</t>
         </is>
       </c>
-      <c r="DO2" s="3" t="inlineStr">
+      <c r="DS2" s="3" t="inlineStr">
         <is>
           <t>EMPLOYER1</t>
         </is>
       </c>
-      <c r="DP2" s="3" t="inlineStr">
+      <c r="DT2" s="3" t="inlineStr">
         <is>
           <t>First</t>
         </is>
       </c>
-      <c r="DQ2" s="3" t="inlineStr">
+      <c r="DU2" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="DR2" s="3" t="inlineStr">
+      <c r="DV2" s="3" t="inlineStr">
         <is>
           <t>9715 EMPLOYER1 AVENUE</t>
         </is>
       </c>
-      <c r="DS2"/>
-      <c r="DT2" s="3" t="inlineStr">
+      <c r="DW2"/>
+      <c r="DX2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="DU2" s="3" t="inlineStr">
+      <c r="DY2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="DV2" s="3" t="inlineStr">
+      <c r="DZ2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="DW2" s="3" t="inlineStr">
+      <c r="EA2" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="DX2" s="3" t="inlineStr">
+      <c r="EB2" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="DY2" s="3" t="inlineStr">
+      <c r="EC2" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="DZ2" s="3" t="inlineStr">
+      <c r="ED2" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="EA2"/>
-      <c r="EB2"/>
-      <c r="EC2"/>
-      <c r="ED2"/>
       <c r="EE2"/>
       <c r="EF2"/>
       <c r="EG2"/>
@@ -2648,56 +2668,56 @@
       <c r="EL2"/>
       <c r="EM2"/>
       <c r="EN2"/>
-      <c r="EO2" s="3" t="inlineStr">
+      <c r="EO2"/>
+      <c r="EP2"/>
+      <c r="EQ2"/>
+      <c r="ER2"/>
+      <c r="ES2" s="3" t="inlineStr">
         <is>
           <t>School1</t>
         </is>
       </c>
-      <c r="EP2" s="3" t="inlineStr">
+      <c r="ET2" s="3" t="inlineStr">
         <is>
           <t>9715 SCHOOL AVENUE</t>
         </is>
       </c>
-      <c r="EQ2"/>
-      <c r="ER2" s="3" t="inlineStr">
+      <c r="EU2"/>
+      <c r="EV2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="ES2" s="3" t="inlineStr">
+      <c r="EW2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="ET2" s="3" t="inlineStr">
+      <c r="EX2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="EU2" s="3" t="inlineStr">
+      <c r="EY2" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="EV2" s="3" t="inlineStr">
+      <c r="EZ2" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="EW2" s="3" t="inlineStr">
+      <c r="FA2" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="EX2" s="3" t="inlineStr">
+      <c r="FB2" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="EY2"/>
-      <c r="EZ2"/>
-      <c r="FA2"/>
-      <c r="FB2"/>
       <c r="FC2"/>
       <c r="FD2"/>
       <c r="FE2"/>
@@ -2705,137 +2725,137 @@
       <c r="FG2"/>
       <c r="FH2"/>
       <c r="FI2"/>
-      <c r="FJ2" s="3" t="inlineStr">
+      <c r="FJ2"/>
+      <c r="FK2"/>
+      <c r="FL2"/>
+      <c r="FM2"/>
+      <c r="FN2" s="3" t="inlineStr">
         <is>
           <t>custodialParentID</t>
         </is>
       </c>
-      <c r="FK2" s="3" t="inlineStr">
+      <c r="FO2" s="3" t="inlineStr">
         <is>
           <t>Custodial</t>
         </is>
       </c>
-      <c r="FL2" s="3" t="inlineStr">
+      <c r="FP2" s="3" t="inlineStr">
         <is>
           <t>Parent</t>
         </is>
       </c>
-      <c r="FM2" s="3" t="inlineStr">
+      <c r="FQ2" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="FN2" s="3" t="inlineStr">
+      <c r="FR2" s="3" t="inlineStr">
         <is>
           <t>9715 CUSTODIAL AVENUE</t>
         </is>
       </c>
-      <c r="FO2"/>
-      <c r="FP2" s="3" t="inlineStr">
+      <c r="FS2"/>
+      <c r="FT2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="FQ2" s="3" t="inlineStr">
+      <c r="FU2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="FR2" s="3" t="inlineStr">
+      <c r="FV2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="FS2" s="3" t="inlineStr">
+      <c r="FW2" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="FT2" s="3" t="inlineStr">
+      <c r="FX2" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="FU2" s="3" t="inlineStr">
+      <c r="FY2" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="FV2" s="3" t="inlineStr">
+      <c r="FZ2" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="FW2" s="3" t="inlineStr">
+      <c r="GA2" s="3" t="inlineStr">
         <is>
           <t>RESPONSIBLE_PARTY</t>
         </is>
       </c>
-      <c r="FX2" s="3" t="inlineStr">
+      <c r="GB2" s="3" t="inlineStr">
         <is>
           <t>responsiblePersonID</t>
         </is>
       </c>
-      <c r="FY2" s="3" t="inlineStr">
+      <c r="GC2" s="3" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
       </c>
-      <c r="FZ2" s="3" t="inlineStr">
+      <c r="GD2" s="3" t="inlineStr">
         <is>
           <t>Person</t>
         </is>
       </c>
-      <c r="GA2" s="3" t="inlineStr">
+      <c r="GE2" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="GB2" s="3" t="inlineStr">
+      <c r="GF2" s="3" t="inlineStr">
         <is>
           <t>9715 RESPONSIBLE AVENUE</t>
         </is>
       </c>
-      <c r="GC2"/>
-      <c r="GD2" s="3" t="inlineStr">
+      <c r="GG2"/>
+      <c r="GH2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="GE2" s="3" t="inlineStr">
+      <c r="GI2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="GF2" s="3" t="inlineStr">
+      <c r="GJ2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="GG2" s="3" t="inlineStr">
+      <c r="GK2" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="GH2" s="3" t="inlineStr">
+      <c r="GL2" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="GI2" s="3" t="inlineStr">
+      <c r="GM2" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="GJ2" s="3" t="inlineStr">
+      <c r="GN2" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="GK2"/>
-      <c r="GL2"/>
-      <c r="GM2"/>
-      <c r="GN2"/>
       <c r="GO2"/>
       <c r="GP2"/>
       <c r="GQ2"/>
@@ -2860,356 +2880,356 @@
       <c r="HJ2"/>
       <c r="HK2"/>
       <c r="HL2"/>
-      <c r="HM2" s="3" t="inlineStr">
-        <is>
-          <t>DropOff</t>
-        </is>
-      </c>
+      <c r="HM2"/>
       <c r="HN2"/>
       <c r="HO2"/>
-      <c r="HP2" s="3" t="inlineStr">
+      <c r="HP2"/>
+      <c r="HQ2" s="3" t="inlineStr">
+        <is>
+          <t>DropOff</t>
+        </is>
+      </c>
+      <c r="HR2"/>
+      <c r="HS2"/>
+      <c r="HT2" s="3" t="inlineStr">
         <is>
           <t>9715 DROPOFF AVENUE</t>
         </is>
       </c>
-      <c r="HQ2"/>
-      <c r="HR2" s="3" t="inlineStr">
+      <c r="HU2"/>
+      <c r="HV2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="HS2" s="3" t="inlineStr">
+      <c r="HW2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="HT2" s="3" t="inlineStr">
+      <c r="HX2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="HU2" s="3" t="inlineStr">
+      <c r="HY2" s="3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="HV2" s="3" t="inlineStr">
+      <c r="HZ2" s="3" t="inlineStr">
         <is>
           <t>585</t>
         </is>
       </c>
-      <c r="HW2" s="4" t="n">
+      <c r="IA2" s="4" t="n">
         <v>45748.0</v>
       </c>
-      <c r="HX2" s="4" t="n">
+      <c r="IB2" s="4" t="n">
         <v>45778.0</v>
       </c>
-      <c r="HY2"/>
-      <c r="HZ2"/>
-      <c r="IA2"/>
-      <c r="IB2"/>
       <c r="IC2"/>
       <c r="ID2"/>
       <c r="IE2"/>
       <c r="IF2"/>
-      <c r="IG2" s="3" t="inlineStr">
+      <c r="IG2"/>
+      <c r="IH2"/>
+      <c r="II2"/>
+      <c r="IJ2"/>
+      <c r="IK2" s="3" t="inlineStr">
         <is>
           <t>SOUTHEASTERN UNION</t>
         </is>
       </c>
-      <c r="IH2" s="3" t="inlineStr">
+      <c r="IL2" s="3" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="II2" s="3" t="inlineStr">
+      <c r="IM2" s="3" t="inlineStr">
         <is>
           <t>UNION_NUMBER</t>
         </is>
       </c>
-      <c r="IJ2" s="3" t="inlineStr">
+      <c r="IN2" s="3" t="inlineStr">
         <is>
           <t>442</t>
         </is>
       </c>
-      <c r="IK2" s="4" t="n">
+      <c r="IO2" s="4" t="n">
         <v>45717.0</v>
       </c>
-      <c r="IL2" s="4" t="n">
+      <c r="IP2" s="4" t="n">
         <v>45808.0</v>
       </c>
-      <c r="IM2" s="3" t="inlineStr">
+      <c r="IQ2" s="3" t="inlineStr">
         <is>
           <t>PAYER2</t>
         </is>
       </c>
-      <c r="IN2" s="3" t="inlineStr">
+      <c r="IR2" s="3" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="IO2" s="3" t="inlineStr">
+      <c r="IS2" s="3" t="inlineStr">
         <is>
           <t>UNION_NUMBER</t>
         </is>
       </c>
-      <c r="IP2" s="3" t="inlineStr">
+      <c r="IT2" s="3" t="inlineStr">
         <is>
           <t>442</t>
         </is>
       </c>
-      <c r="IQ2" s="4" t="n">
+      <c r="IU2" s="4" t="n">
         <v>37987.0</v>
       </c>
-      <c r="IR2"/>
-      <c r="IS2"/>
-      <c r="IT2"/>
-      <c r="IU2"/>
       <c r="IV2"/>
       <c r="IW2"/>
       <c r="IX2"/>
-      <c r="IY2" s="3" t="inlineStr">
+      <c r="IY2"/>
+      <c r="IZ2"/>
+      <c r="JA2"/>
+      <c r="JB2"/>
+      <c r="JC2" s="3" t="inlineStr">
         <is>
           <t>021</t>
         </is>
       </c>
-      <c r="IZ2" s="3" t="inlineStr">
+      <c r="JD2" s="3" t="inlineStr">
         <is>
           <t>HMO</t>
         </is>
       </c>
-      <c r="JA2" s="3" t="inlineStr">
+      <c r="JE2" s="3" t="inlineStr">
         <is>
           <t>PlanDesc</t>
         </is>
       </c>
-      <c r="JB2" s="3" t="inlineStr">
+      <c r="JF2" s="3" t="inlineStr">
         <is>
           <t>FAM</t>
         </is>
       </c>
-      <c r="JC2" s="3" t="inlineStr">
+      <c r="JG2" s="3" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="JD2" s="3" t="inlineStr">
+      <c r="JH2" s="3" t="inlineStr">
         <is>
           <t>348</t>
         </is>
       </c>
-      <c r="JE2" s="4" t="n">
+      <c r="JI2" s="4" t="n">
         <v>35217.0</v>
       </c>
-      <c r="JF2"/>
-      <c r="JG2"/>
-      <c r="JH2"/>
-      <c r="JI2"/>
       <c r="JJ2"/>
       <c r="JK2"/>
       <c r="JL2"/>
       <c r="JM2"/>
-      <c r="JN2" s="3" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="JO2" s="1" t="n">
-        <v>20.0</v>
-      </c>
+      <c r="JN2"/>
+      <c r="JO2"/>
       <c r="JP2"/>
       <c r="JQ2"/>
-      <c r="JR2"/>
-      <c r="JS2"/>
-      <c r="JT2" s="3" t="inlineStr">
-        <is>
-          <t>1L</t>
-        </is>
-      </c>
-      <c r="JU2" s="3" t="inlineStr">
-        <is>
-          <t>PolicyNumber</t>
-        </is>
-      </c>
+      <c r="JR2" s="3" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="JS2" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="JT2"/>
+      <c r="JU2"/>
       <c r="JV2"/>
       <c r="JW2"/>
-      <c r="JX2"/>
-      <c r="JY2"/>
+      <c r="JX2" s="3" t="inlineStr">
+        <is>
+          <t>1L</t>
+        </is>
+      </c>
+      <c r="JY2" s="3" t="inlineStr">
+        <is>
+          <t>PolicyNumber</t>
+        </is>
+      </c>
       <c r="JZ2"/>
       <c r="KA2"/>
       <c r="KB2"/>
       <c r="KC2"/>
-      <c r="KD2" s="3" t="inlineStr">
+      <c r="KD2"/>
+      <c r="KE2"/>
+      <c r="KF2"/>
+      <c r="KG2"/>
+      <c r="KH2" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="KE2" s="3" t="inlineStr">
+      <c r="KI2" s="3" t="inlineStr">
         <is>
           <t>PlanDesc</t>
         </is>
       </c>
-      <c r="KF2" s="3" t="inlineStr">
+      <c r="KJ2" s="3" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="KG2" s="2" t="n">
+      <c r="KK2" s="2" t="n">
         <v>5.0</v>
       </c>
-      <c r="KH2" s="3" t="inlineStr">
+      <c r="KL2" s="3" t="inlineStr">
         <is>
           <t>RX</t>
         </is>
       </c>
-      <c r="KI2" s="3" t="inlineStr">
+      <c r="KM2" s="3" t="inlineStr">
         <is>
           <t>PRIMARY_CARE</t>
         </is>
       </c>
-      <c r="KJ2" s="3" t="inlineStr">
+      <c r="KN2" s="3" t="inlineStr">
         <is>
           <t>INDIVIDUAL</t>
         </is>
       </c>
-      <c r="KK2" s="3" t="inlineStr">
+      <c r="KO2" s="3" t="inlineStr">
         <is>
           <t>prov1ID</t>
         </is>
       </c>
-      <c r="KL2" s="3" t="inlineStr">
+      <c r="KP2" s="3" t="inlineStr">
         <is>
           <t>BROWN</t>
         </is>
       </c>
-      <c r="KM2" s="3" t="inlineStr">
+      <c r="KQ2" s="3" t="inlineStr">
         <is>
           <t>BERNARD</t>
         </is>
       </c>
-      <c r="KN2"/>
-      <c r="KO2" s="3" t="inlineStr">
+      <c r="KR2"/>
+      <c r="KS2" s="3" t="inlineStr">
         <is>
           <t>2715 SOUTHWIND AVENUE</t>
         </is>
       </c>
-      <c r="KP2"/>
-      <c r="KQ2" s="3" t="inlineStr">
+      <c r="KT2"/>
+      <c r="KU2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="KR2" s="3" t="inlineStr">
+      <c r="KV2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="KS2" s="3" t="inlineStr">
+      <c r="KW2" s="3" t="inlineStr">
         <is>
           <t>271110000</t>
         </is>
       </c>
-      <c r="KT2" s="3" t="inlineStr">
+      <c r="KX2" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="KU2" s="3" t="inlineStr">
+      <c r="KY2" s="3" t="inlineStr">
         <is>
           <t>2172343334</t>
         </is>
       </c>
-      <c r="KV2" s="3" t="inlineStr">
+      <c r="KZ2" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="KW2" s="3" t="inlineStr">
+      <c r="LA2" s="3" t="inlineStr">
         <is>
           <t>2172341240</t>
         </is>
       </c>
-      <c r="KX2" s="3" t="inlineStr">
+      <c r="LB2" s="3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="KY2" s="4" t="n">
+      <c r="LC2" s="4" t="n">
         <v>45413.0</v>
       </c>
-      <c r="KZ2" s="3" t="inlineStr">
+      <c r="LD2" s="3" t="inlineStr">
         <is>
           <t>AI</t>
         </is>
       </c>
-      <c r="LA2" s="3" t="inlineStr">
+      <c r="LE2" s="3" t="inlineStr">
         <is>
           <t>MANAGED_CARE</t>
         </is>
       </c>
-      <c r="LB2" s="3" t="inlineStr">
+      <c r="LF2" s="3" t="inlineStr">
         <is>
           <t>INDIVIDUAL</t>
         </is>
       </c>
-      <c r="LC2" s="3" t="inlineStr">
+      <c r="LG2" s="3" t="inlineStr">
         <is>
           <t>943766</t>
         </is>
       </c>
-      <c r="LD2" s="3" t="inlineStr">
+      <c r="LH2" s="3" t="inlineStr">
         <is>
           <t>BROWN</t>
         </is>
       </c>
-      <c r="LE2" s="3" t="inlineStr">
+      <c r="LI2" s="3" t="inlineStr">
         <is>
           <t>BERNARD</t>
         </is>
       </c>
-      <c r="LF2"/>
-      <c r="LG2" s="3" t="inlineStr">
+      <c r="LJ2"/>
+      <c r="LK2" s="3" t="inlineStr">
         <is>
           <t>2715 SOUTHWIND AVENUE</t>
         </is>
       </c>
-      <c r="LH2"/>
-      <c r="LI2" s="3" t="inlineStr">
+      <c r="LL2"/>
+      <c r="LM2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="LJ2" s="3" t="inlineStr">
+      <c r="LN2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="LK2" s="3" t="inlineStr">
+      <c r="LO2" s="3" t="inlineStr">
         <is>
           <t>271110000</t>
         </is>
       </c>
-      <c r="LL2"/>
-      <c r="LM2"/>
-      <c r="LN2"/>
-      <c r="LO2"/>
-      <c r="LP2" s="3" t="inlineStr">
+      <c r="LP2"/>
+      <c r="LQ2"/>
+      <c r="LR2"/>
+      <c r="LS2"/>
+      <c r="LT2" s="3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="LQ2" s="4" t="n">
+      <c r="LU2" s="4" t="n">
         <v>45047.0</v>
       </c>
-      <c r="LR2" s="3" t="inlineStr">
+      <c r="LV2" s="3" t="inlineStr">
         <is>
           <t>AI</t>
         </is>
       </c>
-      <c r="LS2"/>
-      <c r="LT2"/>
-      <c r="LU2"/>
-      <c r="LV2"/>
       <c r="LW2"/>
       <c r="LX2"/>
       <c r="LY2"/>
@@ -3224,112 +3244,112 @@
       <c r="MH2"/>
       <c r="MI2"/>
       <c r="MJ2"/>
-      <c r="MK2" s="3" t="inlineStr">
+      <c r="MK2"/>
+      <c r="ML2"/>
+      <c r="MM2"/>
+      <c r="MN2"/>
+      <c r="MO2" s="3" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="ML2" s="3" t="inlineStr">
+      <c r="MP2" s="3" t="inlineStr">
         <is>
           <t>PRIMARY</t>
         </is>
       </c>
-      <c r="MM2" s="3" t="inlineStr">
+      <c r="MQ2" s="3" t="inlineStr">
         <is>
           <t>XYZ123</t>
         </is>
       </c>
-      <c r="MN2" s="3" t="inlineStr">
+      <c r="MR2" s="3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="MO2" s="3" t="inlineStr">
+      <c r="MS2" s="3" t="inlineStr">
         <is>
           <t>6P</t>
         </is>
       </c>
-      <c r="MP2" s="3" t="inlineStr">
+      <c r="MT2" s="3" t="inlineStr">
         <is>
           <t>COB-GroupNumber</t>
         </is>
       </c>
-      <c r="MQ2" s="3" t="inlineStr">
+      <c r="MU2" s="3" t="inlineStr">
         <is>
           <t>SY</t>
         </is>
       </c>
-      <c r="MR2" s="3" t="inlineStr">
+      <c r="MV2" s="3" t="inlineStr">
         <is>
           <t>COB-SSN</t>
         </is>
       </c>
-      <c r="MS2" s="4" t="n">
+      <c r="MW2" s="4" t="n">
         <v>45689.0</v>
       </c>
-      <c r="MT2" s="4" t="n">
+      <c r="MX2" s="4" t="n">
         <v>45716.0</v>
       </c>
-      <c r="MU2" s="3" t="inlineStr">
+      <c r="MY2" s="3" t="inlineStr">
         <is>
           <t>EMPLOYER</t>
         </is>
       </c>
-      <c r="MV2" s="3" t="inlineStr">
+      <c r="MZ2" s="3" t="inlineStr">
         <is>
           <t>COB-EmployerId</t>
         </is>
       </c>
-      <c r="MW2" s="3" t="inlineStr">
+      <c r="NA2" s="3" t="inlineStr">
         <is>
           <t>COB-Employer</t>
         </is>
       </c>
-      <c r="MX2" s="3" t="inlineStr">
+      <c r="NB2" s="3" t="inlineStr">
         <is>
           <t>9715 RESPONSIBLE AVENUE</t>
         </is>
       </c>
-      <c r="MY2"/>
-      <c r="MZ2" s="3" t="inlineStr">
+      <c r="NC2"/>
+      <c r="ND2" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="NA2" s="3" t="inlineStr">
+      <c r="NE2" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="NB2" s="3" t="inlineStr">
+      <c r="NF2" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="NC2" s="3" t="inlineStr">
+      <c r="NG2" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="ND2" s="3" t="inlineStr">
+      <c r="NH2" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="NE2" s="3" t="inlineStr">
+      <c r="NI2" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="NF2" s="3" t="inlineStr">
+      <c r="NJ2" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="NG2"/>
-      <c r="NH2"/>
-      <c r="NI2"/>
-      <c r="NJ2"/>
       <c r="NK2"/>
       <c r="NL2"/>
       <c r="NM2"/>
@@ -3372,11 +3392,15 @@
       <c r="OX2"/>
       <c r="OY2"/>
       <c r="OZ2"/>
+      <c r="PA2"/>
+      <c r="PB2"/>
+      <c r="PC2"/>
+      <c r="PD2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>684723f4cd41c01c2437b822</t>
+          <t>685d5721e29351212dc46be9</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -3723,147 +3747,147 @@
       <c r="CO3" t="n">
         <v>210.0</v>
       </c>
-      <c r="CP3" s="3" t="inlineStr">
+      <c r="CP3"/>
+      <c r="CQ3"/>
+      <c r="CR3"/>
+      <c r="CS3"/>
+      <c r="CT3" s="3" t="inlineStr">
         <is>
           <t>202443309</t>
         </is>
       </c>
-      <c r="CQ3" s="3" t="inlineStr">
+      <c r="CU3" s="3" t="inlineStr">
         <is>
           <t>DOE</t>
         </is>
       </c>
-      <c r="CR3" s="3" t="inlineStr">
+      <c r="CV3" s="3" t="inlineStr">
         <is>
           <t>JOE</t>
         </is>
       </c>
-      <c r="CS3"/>
-      <c r="CT3" s="4" t="n">
+      <c r="CW3"/>
+      <c r="CX3" s="4" t="n">
         <v>25733.0</v>
       </c>
-      <c r="CU3" s="3" t="inlineStr">
+      <c r="CY3" s="3" t="inlineStr">
         <is>
           <t>MALE</t>
         </is>
       </c>
-      <c r="CV3" s="3" t="inlineStr">
+      <c r="CZ3" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="CW3" s="3" t="inlineStr">
+      <c r="DA3" s="3" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="CX3" s="3" t="inlineStr">
+      <c r="DB3" s="3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="CY3" s="3" t="inlineStr">
+      <c r="DC3" s="3" t="inlineStr">
         <is>
           <t>D2</t>
         </is>
       </c>
-      <c r="CZ3" s="1" t="n">
+      <c r="DD3" s="1" t="n">
         <v>100.0</v>
       </c>
-      <c r="DA3"/>
-      <c r="DB3"/>
-      <c r="DC3"/>
-      <c r="DD3"/>
       <c r="DE3"/>
       <c r="DF3"/>
       <c r="DG3"/>
       <c r="DH3"/>
-      <c r="DI3" s="3" t="inlineStr">
+      <c r="DI3"/>
+      <c r="DJ3"/>
+      <c r="DK3"/>
+      <c r="DL3"/>
+      <c r="DM3" s="3" t="inlineStr">
         <is>
           <t>9715 SOUTHWIND AVENUE</t>
         </is>
       </c>
-      <c r="DJ3"/>
-      <c r="DK3" s="3" t="inlineStr">
+      <c r="DN3"/>
+      <c r="DO3" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="DL3" s="3" t="inlineStr">
+      <c r="DP3" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="DM3" s="3" t="inlineStr">
+      <c r="DQ3" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="DN3" s="3" t="inlineStr">
+      <c r="DR3" s="3" t="inlineStr">
         <is>
           <t>emp1ID</t>
         </is>
       </c>
-      <c r="DO3" s="3" t="inlineStr">
+      <c r="DS3" s="3" t="inlineStr">
         <is>
           <t>EMPLOYER1</t>
         </is>
       </c>
-      <c r="DP3" s="3" t="inlineStr">
+      <c r="DT3" s="3" t="inlineStr">
         <is>
           <t>First</t>
         </is>
       </c>
-      <c r="DQ3" s="3" t="inlineStr">
+      <c r="DU3" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="DR3" s="3" t="inlineStr">
+      <c r="DV3" s="3" t="inlineStr">
         <is>
           <t>9715 EMPLOYER1 AVENUE</t>
         </is>
       </c>
-      <c r="DS3"/>
-      <c r="DT3" s="3" t="inlineStr">
+      <c r="DW3"/>
+      <c r="DX3" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="DU3" s="3" t="inlineStr">
+      <c r="DY3" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="DV3" s="3" t="inlineStr">
+      <c r="DZ3" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="DW3" s="3" t="inlineStr">
+      <c r="EA3" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="DX3" s="3" t="inlineStr">
+      <c r="EB3" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="DY3" s="3" t="inlineStr">
+      <c r="EC3" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="DZ3" s="3" t="inlineStr">
+      <c r="ED3" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="EA3"/>
-      <c r="EB3"/>
-      <c r="EC3"/>
-      <c r="ED3"/>
       <c r="EE3"/>
       <c r="EF3"/>
       <c r="EG3"/>
@@ -3874,56 +3898,56 @@
       <c r="EL3"/>
       <c r="EM3"/>
       <c r="EN3"/>
-      <c r="EO3" s="3" t="inlineStr">
+      <c r="EO3"/>
+      <c r="EP3"/>
+      <c r="EQ3"/>
+      <c r="ER3"/>
+      <c r="ES3" s="3" t="inlineStr">
         <is>
           <t>School1</t>
         </is>
       </c>
-      <c r="EP3" s="3" t="inlineStr">
+      <c r="ET3" s="3" t="inlineStr">
         <is>
           <t>9715 SCHOOL AVENUE</t>
         </is>
       </c>
-      <c r="EQ3"/>
-      <c r="ER3" s="3" t="inlineStr">
+      <c r="EU3"/>
+      <c r="EV3" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="ES3" s="3" t="inlineStr">
+      <c r="EW3" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="ET3" s="3" t="inlineStr">
+      <c r="EX3" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="EU3" s="3" t="inlineStr">
+      <c r="EY3" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="EV3" s="3" t="inlineStr">
+      <c r="EZ3" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="EW3" s="3" t="inlineStr">
+      <c r="FA3" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="EX3" s="3" t="inlineStr">
+      <c r="FB3" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="EY3"/>
-      <c r="EZ3"/>
-      <c r="FA3"/>
-      <c r="FB3"/>
       <c r="FC3"/>
       <c r="FD3"/>
       <c r="FE3"/>
@@ -3931,137 +3955,137 @@
       <c r="FG3"/>
       <c r="FH3"/>
       <c r="FI3"/>
-      <c r="FJ3" s="3" t="inlineStr">
+      <c r="FJ3"/>
+      <c r="FK3"/>
+      <c r="FL3"/>
+      <c r="FM3"/>
+      <c r="FN3" s="3" t="inlineStr">
         <is>
           <t>custodialParentID</t>
         </is>
       </c>
-      <c r="FK3" s="3" t="inlineStr">
+      <c r="FO3" s="3" t="inlineStr">
         <is>
           <t>Custodial</t>
         </is>
       </c>
-      <c r="FL3" s="3" t="inlineStr">
+      <c r="FP3" s="3" t="inlineStr">
         <is>
           <t>Parent</t>
         </is>
       </c>
-      <c r="FM3" s="3" t="inlineStr">
+      <c r="FQ3" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="FN3" s="3" t="inlineStr">
+      <c r="FR3" s="3" t="inlineStr">
         <is>
           <t>9715 CUSTODIAL AVENUE</t>
         </is>
       </c>
-      <c r="FO3"/>
-      <c r="FP3" s="3" t="inlineStr">
+      <c r="FS3"/>
+      <c r="FT3" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="FQ3" s="3" t="inlineStr">
+      <c r="FU3" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="FR3" s="3" t="inlineStr">
+      <c r="FV3" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="FS3" s="3" t="inlineStr">
+      <c r="FW3" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="FT3" s="3" t="inlineStr">
+      <c r="FX3" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="FU3" s="3" t="inlineStr">
+      <c r="FY3" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="FV3" s="3" t="inlineStr">
+      <c r="FZ3" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="FW3" s="3" t="inlineStr">
+      <c r="GA3" s="3" t="inlineStr">
         <is>
           <t>RESPONSIBLE_PARTY</t>
         </is>
       </c>
-      <c r="FX3" s="3" t="inlineStr">
+      <c r="GB3" s="3" t="inlineStr">
         <is>
           <t>responsiblePersonID</t>
         </is>
       </c>
-      <c r="FY3" s="3" t="inlineStr">
+      <c r="GC3" s="3" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
       </c>
-      <c r="FZ3" s="3" t="inlineStr">
+      <c r="GD3" s="3" t="inlineStr">
         <is>
           <t>Person</t>
         </is>
       </c>
-      <c r="GA3" s="3" t="inlineStr">
+      <c r="GE3" s="3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="GB3" s="3" t="inlineStr">
+      <c r="GF3" s="3" t="inlineStr">
         <is>
           <t>9715 RESPONSIBLE AVENUE</t>
         </is>
       </c>
-      <c r="GC3"/>
-      <c r="GD3" s="3" t="inlineStr">
+      <c r="GG3"/>
+      <c r="GH3" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="GE3" s="3" t="inlineStr">
+      <c r="GI3" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="GF3" s="3" t="inlineStr">
+      <c r="GJ3" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="GG3" s="3" t="inlineStr">
+      <c r="GK3" s="3" t="inlineStr">
         <is>
           <t>HOME_PHONE</t>
         </is>
       </c>
-      <c r="GH3" s="3" t="inlineStr">
+      <c r="GL3" s="3" t="inlineStr">
         <is>
           <t>9172343334</t>
         </is>
       </c>
-      <c r="GI3" s="3" t="inlineStr">
+      <c r="GM3" s="3" t="inlineStr">
         <is>
           <t>WORK_PHONE</t>
         </is>
       </c>
-      <c r="GJ3" s="3" t="inlineStr">
+      <c r="GN3" s="3" t="inlineStr">
         <is>
           <t>9172341240</t>
         </is>
       </c>
-      <c r="GK3"/>
-      <c r="GL3"/>
-      <c r="GM3"/>
-      <c r="GN3"/>
       <c r="GO3"/>
       <c r="GP3"/>
       <c r="GQ3"/>
@@ -4086,194 +4110,194 @@
       <c r="HJ3"/>
       <c r="HK3"/>
       <c r="HL3"/>
-      <c r="HM3" s="3" t="inlineStr">
-        <is>
-          <t>DropOff</t>
-        </is>
-      </c>
+      <c r="HM3"/>
       <c r="HN3"/>
       <c r="HO3"/>
-      <c r="HP3" s="3" t="inlineStr">
+      <c r="HP3"/>
+      <c r="HQ3" s="3" t="inlineStr">
+        <is>
+          <t>DropOff</t>
+        </is>
+      </c>
+      <c r="HR3"/>
+      <c r="HS3"/>
+      <c r="HT3" s="3" t="inlineStr">
         <is>
           <t>9715 DROPOFF AVENUE</t>
         </is>
       </c>
-      <c r="HQ3"/>
-      <c r="HR3" s="3" t="inlineStr">
+      <c r="HU3"/>
+      <c r="HV3" s="3" t="inlineStr">
         <is>
           <t>ANYTOWN</t>
         </is>
       </c>
-      <c r="HS3" s="3" t="inlineStr">
+      <c r="HW3" s="3" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
-      <c r="HT3" s="3" t="inlineStr">
+      <c r="HX3" s="3" t="inlineStr">
         <is>
           <t>971110000</t>
         </is>
       </c>
-      <c r="HU3" s="3" t="inlineStr">
+      <c r="HY3" s="3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="HV3" s="3" t="inlineStr">
+      <c r="HZ3" s="3" t="inlineStr">
         <is>
           <t>585</t>
         </is>
       </c>
-      <c r="HW3" s="4" t="n">
+      <c r="IA3" s="4" t="n">
         <v>45748.0</v>
       </c>
-      <c r="HX3" s="4" t="n">
+      <c r="IB3" s="4" t="n">
         <v>45778.0</v>
       </c>
-      <c r="HY3"/>
-      <c r="HZ3"/>
-      <c r="IA3"/>
-      <c r="IB3"/>
       <c r="IC3"/>
       <c r="ID3"/>
       <c r="IE3"/>
       <c r="IF3"/>
-      <c r="IG3" s="3" t="inlineStr">
+      <c r="IG3"/>
+      <c r="IH3"/>
+      <c r="II3"/>
+      <c r="IJ3"/>
+      <c r="IK3" s="3" t="inlineStr">
         <is>
           <t>SOUTHEASTERN UNION</t>
         </is>
       </c>
-      <c r="IH3" s="3" t="inlineStr">
+      <c r="IL3" s="3" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="II3" s="3" t="inlineStr">
+      <c r="IM3" s="3" t="inlineStr">
         <is>
           <t>UNION_NUMBER</t>
         </is>
       </c>
-      <c r="IJ3" s="3" t="inlineStr">
+      <c r="IN3" s="3" t="inlineStr">
         <is>
           <t>442</t>
         </is>
       </c>
-      <c r="IK3" s="4" t="n">
+      <c r="IO3" s="4" t="n">
         <v>45717.0</v>
       </c>
-      <c r="IL3" s="4" t="n">
+      <c r="IP3" s="4" t="n">
         <v>45808.0</v>
       </c>
-      <c r="IM3" s="3" t="inlineStr">
+      <c r="IQ3" s="3" t="inlineStr">
         <is>
           <t>PAYER2</t>
         </is>
       </c>
-      <c r="IN3" s="3" t="inlineStr">
+      <c r="IR3" s="3" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="IO3" s="3" t="inlineStr">
+      <c r="IS3" s="3" t="inlineStr">
         <is>
           <t>UNION_NUMBER</t>
         </is>
       </c>
-      <c r="IP3" s="3" t="inlineStr">
+      <c r="IT3" s="3" t="inlineStr">
         <is>
           <t>442</t>
         </is>
       </c>
-      <c r="IQ3" s="4" t="n">
+      <c r="IU3" s="4" t="n">
         <v>37987.0</v>
       </c>
-      <c r="IR3"/>
-      <c r="IS3"/>
-      <c r="IT3"/>
-      <c r="IU3"/>
       <c r="IV3"/>
       <c r="IW3"/>
       <c r="IX3"/>
-      <c r="IY3" s="3" t="inlineStr">
+      <c r="IY3"/>
+      <c r="IZ3"/>
+      <c r="JA3"/>
+      <c r="JB3"/>
+      <c r="JC3" s="3" t="inlineStr">
         <is>
           <t>021</t>
         </is>
       </c>
-      <c r="IZ3" s="3" t="inlineStr">
+      <c r="JD3" s="3" t="inlineStr">
         <is>
           <t>EPO</t>
         </is>
       </c>
-      <c r="JA3" s="3" t="inlineStr">
+      <c r="JE3" s="3" t="inlineStr">
         <is>
           <t>PlanDesc2</t>
         </is>
       </c>
-      <c r="JB3" s="3" t="inlineStr">
+      <c r="JF3" s="3" t="inlineStr">
         <is>
           <t>FAM</t>
         </is>
       </c>
-      <c r="JC3" s="3" t="inlineStr">
+      <c r="JG3" s="3" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="JD3" s="3" t="inlineStr">
+      <c r="JH3" s="3" t="inlineStr">
         <is>
           <t>348</t>
         </is>
       </c>
-      <c r="JE3" s="4" t="n">
+      <c r="JI3" s="4" t="n">
         <v>45778.0</v>
       </c>
-      <c r="JF3"/>
-      <c r="JG3"/>
-      <c r="JH3"/>
-      <c r="JI3"/>
       <c r="JJ3"/>
       <c r="JK3"/>
       <c r="JL3"/>
       <c r="JM3"/>
-      <c r="JN3" s="3" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="JO3" s="1" t="n">
-        <v>20.0</v>
-      </c>
+      <c r="JN3"/>
+      <c r="JO3"/>
       <c r="JP3"/>
       <c r="JQ3"/>
-      <c r="JR3"/>
-      <c r="JS3"/>
-      <c r="JT3" s="3" t="inlineStr">
-        <is>
-          <t>1L</t>
-        </is>
-      </c>
-      <c r="JU3" s="3" t="inlineStr">
-        <is>
-          <t>PolicyNumber2</t>
-        </is>
-      </c>
+      <c r="JR3" s="3" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="JS3" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="JT3"/>
+      <c r="JU3"/>
       <c r="JV3"/>
       <c r="JW3"/>
-      <c r="JX3"/>
-      <c r="JY3"/>
+      <c r="JX3" s="3" t="inlineStr">
+        <is>
+          <t>1L</t>
+        </is>
+      </c>
+      <c r="JY3" s="3" t="inlineStr">
+        <is>
+          <t>PolicyNumber2</t>
+        </is>
+      </c>
       <c r="JZ3"/>
       <c r="KA3"/>
       <c r="KB3"/>
       <c r="KC3"/>
-      <c r="KD3" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="KD3"/>
       <c r="KE3"/>
       <c r="KF3"/>
       <c r="KG3"/>
-      <c r="KH3"/>
+      <c r="KH3" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="KI3"/>
       <c r="KJ3"/>
       <c r="KK3"/>
@@ -4396,11 +4420,15 @@
       <c r="OX3"/>
       <c r="OY3"/>
       <c r="OZ3"/>
+      <c r="PA3"/>
+      <c r="PB3"/>
+      <c r="PC3"/>
+      <c r="PD3"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>684723f4cd41c01c2437b823</t>
+          <t>685d5721e29351212dc46bea</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -4836,31 +4864,31 @@
       <c r="IV4"/>
       <c r="IW4"/>
       <c r="IX4"/>
-      <c r="IY4" s="3" t="inlineStr">
-        <is>
-          <t>021</t>
-        </is>
-      </c>
-      <c r="IZ4" s="3" t="inlineStr">
-        <is>
-          <t>HMO</t>
-        </is>
-      </c>
+      <c r="IY4"/>
+      <c r="IZ4"/>
       <c r="JA4"/>
       <c r="JB4"/>
-      <c r="JC4"/>
+      <c r="JC4" s="3" t="inlineStr">
+        <is>
+          <t>021</t>
+        </is>
+      </c>
       <c r="JD4" s="3" t="inlineStr">
         <is>
-          <t>348</t>
-        </is>
-      </c>
-      <c r="JE4" s="4" t="n">
-        <v>35217.0</v>
-      </c>
+          <t>HMO</t>
+        </is>
+      </c>
+      <c r="JE4"/>
       <c r="JF4"/>
       <c r="JG4"/>
-      <c r="JH4"/>
-      <c r="JI4"/>
+      <c r="JH4" s="3" t="inlineStr">
+        <is>
+          <t>348</t>
+        </is>
+      </c>
+      <c r="JI4" s="4" t="n">
+        <v>35217.0</v>
+      </c>
       <c r="JJ4"/>
       <c r="JK4"/>
       <c r="JL4"/>
@@ -4886,58 +4914,58 @@
       <c r="KF4"/>
       <c r="KG4"/>
       <c r="KH4"/>
-      <c r="KI4" s="3" t="inlineStr">
+      <c r="KI4"/>
+      <c r="KJ4"/>
+      <c r="KK4"/>
+      <c r="KL4"/>
+      <c r="KM4" s="3" t="inlineStr">
         <is>
           <t>PRIMARY_CARE</t>
         </is>
       </c>
-      <c r="KJ4" s="3" t="inlineStr">
+      <c r="KN4" s="3" t="inlineStr">
         <is>
           <t>INDIVIDUAL</t>
         </is>
       </c>
-      <c r="KK4" s="3" t="inlineStr">
+      <c r="KO4" s="3" t="inlineStr">
         <is>
           <t>143766</t>
         </is>
       </c>
-      <c r="KL4" s="3" t="inlineStr">
+      <c r="KP4" s="3" t="inlineStr">
         <is>
           <t>BROWN</t>
         </is>
       </c>
-      <c r="KM4" s="3" t="inlineStr">
+      <c r="KQ4" s="3" t="inlineStr">
         <is>
           <t>BERNARD</t>
         </is>
       </c>
-      <c r="KN4"/>
-      <c r="KO4"/>
-      <c r="KP4"/>
-      <c r="KQ4"/>
       <c r="KR4"/>
       <c r="KS4"/>
       <c r="KT4"/>
       <c r="KU4"/>
       <c r="KV4"/>
       <c r="KW4"/>
-      <c r="KX4" s="3" t="inlineStr">
+      <c r="KX4"/>
+      <c r="KY4"/>
+      <c r="KZ4"/>
+      <c r="LA4"/>
+      <c r="LB4" s="3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="KY4" s="4" t="n">
+      <c r="LC4" s="4" t="n">
         <v>45413.0</v>
       </c>
-      <c r="KZ4" s="3" t="inlineStr">
+      <c r="LD4" s="3" t="inlineStr">
         <is>
           <t>AI</t>
         </is>
       </c>
-      <c r="LA4"/>
-      <c r="LB4"/>
-      <c r="LC4"/>
-      <c r="LD4"/>
       <c r="LE4"/>
       <c r="LF4"/>
       <c r="LG4"/>
@@ -5038,11 +5066,15 @@
       <c r="OX4"/>
       <c r="OY4"/>
       <c r="OZ4"/>
+      <c r="PA4"/>
+      <c r="PB4"/>
+      <c r="PC4"/>
+      <c r="PD4"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>684723f4cd41c01c2437b824</t>
+          <t>685d5721e29351212dc46beb</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -5306,18 +5338,18 @@
       <c r="CV5"/>
       <c r="CW5"/>
       <c r="CX5"/>
-      <c r="CY5" s="3" t="inlineStr">
-        <is>
-          <t>D2</t>
-        </is>
-      </c>
-      <c r="CZ5" s="1" t="n">
-        <v>100.0</v>
-      </c>
+      <c r="CY5"/>
+      <c r="CZ5"/>
       <c r="DA5"/>
       <c r="DB5"/>
-      <c r="DC5"/>
-      <c r="DD5"/>
+      <c r="DC5" s="3" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+      <c r="DD5" s="1" t="n">
+        <v>100.0</v>
+      </c>
       <c r="DE5"/>
       <c r="DF5"/>
       <c r="DG5"/>
@@ -5626,6 +5658,10 @@
       <c r="OX5"/>
       <c r="OY5"/>
       <c r="OZ5"/>
+      <c r="PA5"/>
+      <c r="PB5"/>
+      <c r="PC5"/>
+      <c r="PD5"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Updated converted files examples
</commit_message>
<xml_diff>
--- a/converted_files/834/834-all-fields.xlsx
+++ b/converted_files/834/834-all-fields.xlsx
@@ -2170,7 +2170,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>685d5721e29351212dc46be9</t>
+          <t>690141eb7c0fb18b049a02d7</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -3400,7 +3400,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>685d5721e29351212dc46be9</t>
+          <t>690141eb7c0fb18b049a02d7</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -4428,7 +4428,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>685d5721e29351212dc46bea</t>
+          <t>690141eb7c0fb18b049a02d8</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -5074,7 +5074,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>685d5721e29351212dc46beb</t>
+          <t>690141eb7c0fb18b049a02d9</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">

</xml_diff>